<commit_message>
sr: add oem form
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Sierra Leone/sr_oncho_oem_2_participant_202211.xlsx
+++ b/ONCHO/OEM/Sierra Leone/sr_oncho_oem_2_participant_202211.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\OEM\Sierra Leone\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C606FAC-355E-4BB9-947B-682AEF54337F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12240" tabRatio="500"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>type</t>
   </si>
@@ -165,9 +171,6 @@
     <t>Please select the gender</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>p_age_yrs</t>
   </si>
   <si>
@@ -264,26 +267,20 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Avr 2022) OEM - 2. Participant Form</t>
-  </si>
-  <si>
-    <t>ng_oncho_oem_2_participant_202204</t>
-  </si>
-  <si>
     <t>French</t>
+  </si>
+  <si>
+    <t>sr_oncho_oem_2_participant_202211</t>
+  </si>
+  <si>
+    <t>(Nov 2022) OEM - 2. Participant Form</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,7 +293,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -304,169 +301,25 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,194 +332,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -706,266 +373,24 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </left>
       <right style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </right>
       <top style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </top>
       <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+        <color theme="0" tint="-0.14993743705557422"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1005,62 +430,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1318,40 +702,39 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="19.6296296296296" customWidth="1"/>
-    <col min="2" max="2" width="20.3333333333333" customWidth="1"/>
-    <col min="3" max="3" width="47.5037037037037" customWidth="1"/>
-    <col min="4" max="4" width="47.3703703703704" customWidth="1"/>
-    <col min="5" max="5" width="12.6296296296296" customWidth="1"/>
+    <col min="1" max="1" width="19.609375" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="47.5" customWidth="1"/>
+    <col min="4" max="4" width="47.38671875" customWidth="1"/>
+    <col min="5" max="5" width="12.609375" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="37.7777777777778" customWidth="1"/>
-    <col min="8" max="8" width="20.3703703703704" customWidth="1"/>
-    <col min="9" max="9" width="12.6296296296296" customWidth="1"/>
-    <col min="10" max="10" width="9.75555555555556" customWidth="1"/>
-    <col min="11" max="11" width="35.3703703703704" customWidth="1"/>
-    <col min="12" max="12" width="13.8740740740741" customWidth="1"/>
-    <col min="13" max="13" width="36.6296296296296" customWidth="1"/>
+    <col min="7" max="7" width="37.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.38671875" customWidth="1"/>
+    <col min="9" max="9" width="12.609375" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" customWidth="1"/>
+    <col min="11" max="11" width="35.38671875" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="36.609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="1" ht="18" spans="1:14">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="18">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1395,7 +778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" s="3" customFormat="1" spans="1:13">
+    <row r="2" spans="1:14" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1424,7 +807,7 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" s="3" customFormat="1" spans="1:12">
+    <row r="3" spans="1:14" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1445,7 +828,7 @@
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
     </row>
-    <row r="4" s="3" customFormat="1" spans="1:12">
+    <row r="4" spans="1:14" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1466,7 +849,7 @@
       <c r="K4" s="15"/>
       <c r="L4" s="15"/>
     </row>
-    <row r="5" s="3" customFormat="1" spans="1:13">
+    <row r="5" spans="1:14" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1489,7 +872,7 @@
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" s="3" customFormat="1" spans="1:13">
+    <row r="6" spans="1:14" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
@@ -1510,7 +893,7 @@
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:13">
+    <row r="7" spans="1:14" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -1533,7 +916,7 @@
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1556,7 +939,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:10">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1579,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:14">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1602,7 +985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" s="13" customFormat="1" ht="15.75" customHeight="1" spans="1:14">
+    <row r="11" spans="1:14" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>46</v>
       </c>
@@ -1626,26 +1009,23 @@
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
-      <c r="N11" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:10">
+    </row>
+    <row r="12" spans="1:14" s="3" customFormat="1">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>51</v>
       </c>
       <c r="D12" s="17"/>
       <c r="F12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>38</v>
@@ -1654,15 +1034,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>38</v>
@@ -1671,446 +1051,443 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c r="C15" t="s">
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>63</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
       </c>
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
         <v>65</v>
       </c>
-      <c r="B17" t="s">
-        <v>66</v>
-      </c>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="10:10">
+    <row r="18" spans="1:10">
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="10:10">
+    <row r="19" spans="1:10">
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="10:10">
+    <row r="20" spans="1:10">
       <c r="J20" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="16.3703703703704" customWidth="1"/>
-    <col min="2" max="2" width="39.6296296296296" customWidth="1"/>
-    <col min="3" max="3" width="23.7555555555556" customWidth="1"/>
-    <col min="4" max="4" width="11.7555555555556" customWidth="1"/>
+    <col min="1" max="1" width="16.38671875" customWidth="1"/>
+    <col min="2" max="2" width="39.609375" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="11"/>
+    </row>
+    <row r="2" spans="1:5" s="4" customFormat="1">
+      <c r="A2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" s="4" customFormat="1" spans="1:5">
-      <c r="A2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" s="4" customFormat="1" spans="1:5">
+    <row r="3" spans="1:5" s="4" customFormat="1">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" s="4" customFormat="1" spans="1:5">
+    <row r="4" spans="1:5" s="4" customFormat="1">
       <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>74</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" s="4" customFormat="1" spans="1:5">
+    <row r="5" spans="1:5" s="4" customFormat="1">
       <c r="A5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" s="4" customFormat="1" spans="1:5">
+    <row r="6" spans="1:5" s="4" customFormat="1">
       <c r="A6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>77</v>
-      </c>
       <c r="C6" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="7" s="4" customFormat="1" spans="1:5">
+    <row r="7" spans="1:5" s="4" customFormat="1">
       <c r="A7" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" s="4" customFormat="1" spans="1:5">
+    <row r="8" spans="1:5" s="4" customFormat="1">
       <c r="A8" s="7"/>
       <c r="B8" s="10"/>
       <c r="C8" s="9"/>
       <c r="D8" s="7"/>
       <c r="E8" s="12"/>
     </row>
-    <row r="9" s="4" customFormat="1" spans="1:5">
+    <row r="9" spans="1:5" s="4" customFormat="1">
       <c r="A9" s="7"/>
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
       <c r="D9" s="7"/>
       <c r="E9" s="12"/>
     </row>
-    <row r="10" s="4" customFormat="1" spans="1:5">
+    <row r="10" spans="1:5" s="4" customFormat="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
       <c r="D10" s="7"/>
       <c r="E10" s="12"/>
     </row>
-    <row r="11" s="4" customFormat="1" spans="1:5">
+    <row r="11" spans="1:5" s="4" customFormat="1">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
       <c r="D11" s="7"/>
       <c r="E11" s="12"/>
     </row>
-    <row r="12" s="4" customFormat="1" spans="1:5">
+    <row r="12" spans="1:5" s="4" customFormat="1">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="9"/>
       <c r="D12" s="7"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" s="4" customFormat="1" spans="1:5">
+    <row r="13" spans="1:5" s="4" customFormat="1">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
       <c r="D13" s="7"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" s="4" customFormat="1" spans="1:5">
+    <row r="14" spans="1:5" s="4" customFormat="1">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
       <c r="D14" s="7"/>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" s="4" customFormat="1" spans="1:5">
+    <row r="15" spans="1:5" s="4" customFormat="1">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
       <c r="D15" s="7"/>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" s="4" customFormat="1" spans="1:5">
+    <row r="16" spans="1:5" s="4" customFormat="1">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
       <c r="D16" s="7"/>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" s="4" customFormat="1" spans="1:5">
+    <row r="17" spans="1:5" s="4" customFormat="1">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
       <c r="D17" s="7"/>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" s="4" customFormat="1" spans="1:5">
+    <row r="18" spans="1:5" s="4" customFormat="1">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
       <c r="D18" s="7"/>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" s="4" customFormat="1" spans="1:5">
+    <row r="19" spans="1:5" s="4" customFormat="1">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
       <c r="D19" s="7"/>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" s="4" customFormat="1" spans="1:5">
+    <row r="20" spans="1:5" s="4" customFormat="1">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
       <c r="D20" s="7"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" s="4" customFormat="1" spans="1:5">
+    <row r="21" spans="1:5" s="4" customFormat="1">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" s="4" customFormat="1" spans="1:5">
+    <row r="22" spans="1:5" s="4" customFormat="1">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
       <c r="D22" s="7"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" s="4" customFormat="1" spans="1:5">
+    <row r="23" spans="1:5" s="4" customFormat="1">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
       <c r="D23" s="7"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" s="4" customFormat="1" spans="1:5">
+    <row r="24" spans="1:5" s="4" customFormat="1">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
       <c r="D24" s="7"/>
       <c r="E24" s="12"/>
     </row>
-    <row r="25" s="4" customFormat="1" spans="1:5">
+    <row r="25" spans="1:5" s="4" customFormat="1">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
       <c r="D25" s="7"/>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" s="4" customFormat="1" spans="1:5">
+    <row r="26" spans="1:5" s="4" customFormat="1">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="9"/>
       <c r="D26" s="7"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" s="4" customFormat="1" spans="1:5">
+    <row r="27" spans="1:5" s="4" customFormat="1">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="9"/>
       <c r="D27" s="7"/>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" s="4" customFormat="1" spans="1:5">
+    <row r="28" spans="1:5" s="4" customFormat="1">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="9"/>
       <c r="D28" s="7"/>
       <c r="E28" s="12"/>
     </row>
-    <row r="29" s="4" customFormat="1" spans="1:5">
+    <row r="29" spans="1:5" s="4" customFormat="1">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="9"/>
       <c r="D29" s="7"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" s="4" customFormat="1" spans="1:5">
+    <row r="30" spans="1:5" s="4" customFormat="1">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="9"/>
       <c r="D30" s="7"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" s="4" customFormat="1" spans="1:5">
+    <row r="31" spans="1:5" s="4" customFormat="1">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="9"/>
       <c r="D31" s="7"/>
       <c r="E31" s="12"/>
     </row>
-    <row r="32" s="4" customFormat="1" spans="1:5">
+    <row r="32" spans="1:5" s="4" customFormat="1">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
       <c r="D32" s="7"/>
       <c r="E32" s="12"/>
     </row>
-    <row r="33" s="4" customFormat="1" spans="1:5">
+    <row r="33" spans="1:5" s="4" customFormat="1">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="9"/>
       <c r="D33" s="7"/>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" s="4" customFormat="1" spans="1:5">
+    <row r="34" spans="1:5" s="4" customFormat="1">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="9"/>
       <c r="D34" s="7"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" s="4" customFormat="1" spans="1:5">
+    <row r="35" spans="1:5" s="4" customFormat="1">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="9"/>
       <c r="D35" s="7"/>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" s="4" customFormat="1" spans="1:5">
+    <row r="36" spans="1:5" s="4" customFormat="1">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="9"/>
       <c r="D36" s="7"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" s="4" customFormat="1" spans="1:5">
+    <row r="37" spans="1:5" s="4" customFormat="1">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="9"/>
       <c r="D37" s="7"/>
       <c r="E37" s="12"/>
     </row>
-    <row r="38" s="4" customFormat="1" spans="1:5">
+    <row r="38" spans="1:5" s="4" customFormat="1">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="9"/>
       <c r="D38" s="7"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" s="4" customFormat="1" spans="1:5">
+    <row r="39" spans="1:5" s="4" customFormat="1">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="9"/>
       <c r="D39" s="7"/>
       <c r="E39" s="12"/>
     </row>
-    <row r="40" s="4" customFormat="1" spans="1:5">
+    <row r="40" spans="1:5" s="4" customFormat="1">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="9"/>
       <c r="D40" s="7"/>
       <c r="E40" s="12"/>
     </row>
-    <row r="41" s="4" customFormat="1" spans="1:5">
+    <row r="41" spans="1:5" s="4" customFormat="1">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="9"/>
       <c r="D41" s="7"/>
       <c r="E41" s="12"/>
     </row>
-    <row r="42" s="4" customFormat="1" spans="1:5">
+    <row r="42" spans="1:5" s="4" customFormat="1">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="9"/>
       <c r="D42" s="7"/>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" s="4" customFormat="1" spans="1:5">
+    <row r="43" spans="1:5" s="4" customFormat="1">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="9"/>
       <c r="D43" s="7"/>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" s="4" customFormat="1" spans="1:5">
+    <row r="44" spans="1:5" s="4" customFormat="1">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="9"/>
       <c r="D44" s="7"/>
       <c r="E44" s="12"/>
     </row>
-    <row r="45" s="4" customFormat="1" spans="1:5">
+    <row r="45" spans="1:5" s="4" customFormat="1">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="9"/>
       <c r="D45" s="7"/>
       <c r="E45" s="12"/>
     </row>
-    <row r="46" s="4" customFormat="1" spans="1:5">
+    <row r="46" spans="1:5" s="4" customFormat="1">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="9"/>
@@ -2118,54 +1495,51 @@
       <c r="E46" s="12"/>
     </row>
   </sheetData>
-  <sortState ref="A10:E46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:E46">
     <sortCondition ref="B10:B46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7"/>
   <cols>
-    <col min="1" max="1" width="46.1259259259259" customWidth="1"/>
-    <col min="2" max="2" width="33.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>